<commit_message>
Update Simulink Test Results.xlsx
</commit_message>
<xml_diff>
--- a/Test Results/Simulink Test Results.xlsx
+++ b/Test Results/Simulink Test Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07b0391834ff6c23/Documents/MATLAB/Software Defined Networking (SDN) ^0 Radio (SDR)/SDR_KSU/Matlab Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07b0391834ff6c23/Documents/MATLAB/Software Defined Networking (SDN) ^0 Radio (SDR)/SDR_KSU/Test Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="11_F25DC773A252ABDACC104845019F66A25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{282539ED-A8A4-4776-9804-AED234B97FDD}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="11_F25DC773A252ABDACC104845019F66A25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F076C959-A59B-4BE9-B978-D6B48A31B416}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,12 +212,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -245,6 +239,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,8 +1198,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>4594411</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3573113</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>5568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2419,173 +2419,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="70" style="4" customWidth="1"/>
-    <col min="5" max="5" width="69.5703125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="70.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70" style="2" customWidth="1"/>
+    <col min="5" max="5" width="69.5703125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="70.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="297" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:8" ht="309.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="285" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="285.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="10" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="283.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="10" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="281.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="281.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="10" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="285" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="10" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+      <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to add Project Report.
</commit_message>
<xml_diff>
--- a/Test Results/Simulink Test Results.xlsx
+++ b/Test Results/Simulink Test Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="331" documentId="11_F25DC773A252ABDACC104845019F66A25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F076C959-A59B-4BE9-B978-D6B48A31B416}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Results" sheetId="1" r:id="rId1"/>
@@ -2420,7 +2420,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>

</xml_diff>